<commit_message>
more cleaning and (re)moving of files
</commit_message>
<xml_diff>
--- a/felkla/2_preproc/epi_readout_par.xlsx
+++ b/felkla/2_preproc/epi_readout_par.xlsx
@@ -21,52 +21,67 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
-  <si>
-    <t>echo spacing</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
   <si>
     <t>Base resolution</t>
   </si>
   <si>
-    <t>Grappa</t>
-  </si>
-  <si>
     <t>Partial Fourier</t>
   </si>
   <si>
-    <t>read out</t>
-  </si>
-  <si>
-    <t>How to calculate:</t>
-  </si>
-  <si>
-    <t>Number of line * echo spacing</t>
-  </si>
-  <si>
-    <t>however, this changes when using acceleration</t>
-  </si>
-  <si>
-    <t>cmrr_2iso_mb6_TR945_skyra_shortEcho_EH</t>
-  </si>
-  <si>
-    <t>ANGER</t>
-  </si>
-  <si>
-    <t>no GRAPPA used??</t>
-  </si>
-  <si>
-    <t>AA-Freeze</t>
-  </si>
-  <si>
-    <t>cmrr_2p0iso_mb4_TR1500</t>
+    <t>TELOS</t>
+  </si>
+  <si>
+    <t>Echo spacing</t>
+  </si>
+  <si>
+    <t>Protocol</t>
+  </si>
+  <si>
+    <t>ninEPI_bold_v12C (mb2, TR1975, TE26)</t>
+  </si>
+  <si>
+    <t>&lt;your protocol&gt;</t>
+  </si>
+  <si>
+    <t>EPI read out</t>
+  </si>
+  <si>
+    <t>ms</t>
+  </si>
+  <si>
+    <t>1 = no acc.</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Corrected resolution</t>
+  </si>
+  <si>
+    <t>&lt;your study&gt;</t>
+  </si>
+  <si>
+    <t>(range 1 - 8)</t>
+  </si>
+  <si>
+    <t>part four.</t>
+  </si>
+  <si>
+    <t>grappa</t>
+  </si>
+  <si>
+    <t>GRAPPA AF</t>
+  </si>
+  <si>
+    <t>(read-out px)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -89,8 +104,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -99,18 +122,30 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC00000"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -127,19 +162,172 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -446,10 +634,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -457,144 +645,178 @@
     <col min="1" max="1" width="48" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" customWidth="1"/>
-    <col min="9" max="9" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" customWidth="1"/>
+    <col min="6" max="6" width="14" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="15"/>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="4"/>
+      <c r="B2" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="24" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="6"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="8">
+        <v>0.6</v>
+      </c>
+      <c r="C4" s="8">
+        <v>112</v>
+      </c>
+      <c r="D4" s="8">
+        <v>1</v>
+      </c>
+      <c r="E4" s="8">
         <v>8</v>
       </c>
-      <c r="B5">
-        <v>0.77</v>
-      </c>
-      <c r="C5">
-        <v>104</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5">
+      <c r="F4" s="9">
+        <f>C4*(E4/8)</f>
+        <v>112</v>
+      </c>
+      <c r="G4" s="7">
+        <f>ROUNDUP(F4/D4,0)</f>
+        <v>112</v>
+      </c>
+      <c r="H4" s="10">
+        <f>G4*B4</f>
+        <v>67.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="11"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="18"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="19"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="3">
-        <f>C5*(E5/8)</f>
-        <v>78</v>
-      </c>
-      <c r="G5" s="3">
-        <f>ROUNDUP(F5/D5,0)</f>
-        <v>78</v>
-      </c>
-      <c r="H5" s="3">
-        <f>G5*B5</f>
-        <v>60.06</v>
-      </c>
-      <c r="I5" t="s">
+      <c r="B7" s="8" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8">
-        <v>0.54</v>
-      </c>
-      <c r="C8">
-        <v>104</v>
-      </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-      <c r="E8">
-        <v>7</v>
-      </c>
-      <c r="F8" s="3">
-        <f>C8*(E8/8)</f>
-        <v>91</v>
-      </c>
-      <c r="G8" s="3">
-        <f>ROUNDUP(F8/D8,0)</f>
-        <v>91</v>
-      </c>
-      <c r="H8" s="3">
-        <f>G8*B8</f>
-        <v>49.14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
+      <c r="C7" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="17" t="e">
+        <f>C7*(E7/8)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G7" s="10" t="e">
+        <f>ROUNDUP(F7/D7,0)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H7" s="10" t="e">
+        <f>G7*B7</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="13"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A4:H4"/>
-    <mergeCell ref="A7:H7"/>
+  <mergeCells count="3">
+    <mergeCell ref="A6:H6"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="F1:G1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="141" orientation="portrait" r:id="rId1"/>

</xml_diff>